<commit_message>
Finalizada automação referente ao desafio Deanta Global
</commit_message>
<xml_diff>
--- a/docs/cenarios_teste.xlsx
+++ b/docs/cenarios_teste.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="test_scenario" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
   <si>
     <t>ID</t>
   </si>
@@ -347,13 +347,74 @@
   </si>
   <si>
     <t>Pesquisar usuário por id</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enviar GET para </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/usuarios/_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Retorno HTTP 200 OK com mensagem  "Usuário encontrado" e o json com as chaves e valores do usuário.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deletar usuário por id </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enviar DELETE para </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/usuarios/_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Retorno HTTP 200 OK com mensagem  "Registro excluído com sucesso" .</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,14 +432,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -467,7 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -806,23 +859,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" customWidth="1"/>
+    <col min="4" max="4" width="36.109375" customWidth="1"/>
+    <col min="5" max="5" width="28.44140625" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -836,7 +889,7 @@
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -850,7 +903,7 @@
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -876,7 +929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>20</v>
       </c>
@@ -902,7 +955,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
@@ -918,15 +971,17 @@
       <c r="E8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="G8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -942,15 +997,17 @@
       <c r="E9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="G9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -966,15 +1023,17 @@
       <c r="E10" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="G10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -990,15 +1049,17 @@
       <c r="E11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="G11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1014,15 +1075,17 @@
       <c r="E12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="G12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>26</v>
       </c>
@@ -1038,15 +1101,17 @@
       <c r="E13" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="G13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>27</v>
       </c>
@@ -1056,25 +1121,49 @@
       <c r="C14" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>29</v>
       </c>
@@ -1086,7 +1175,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>30</v>
       </c>
@@ -1098,7 +1187,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>31</v>
       </c>
@@ -1154,7 +1243,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1168,12 +1257,12 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -1184,7 +1273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1195,7 +1284,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1206,7 +1295,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>14</v>
       </c>
@@ -1214,12 +1303,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>19</v>
       </c>

</xml_diff>